<commit_message>
finalizando planilha de arquitetura
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de arquitetura.xlsx
+++ b/Documentação/Planilha de arquitetura.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD07100-6FC4-44C0-95B4-D4A1DF5E28A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CBBE3F-8E1F-45BE-A5D2-3953200CD16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guia de Engenharia v4" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>O que é crítico na sua aplicação? O que gera alto impacto?</t>
   </si>
@@ -103,9 +101,6 @@
     <t>Deploy</t>
   </si>
   <si>
-    <t>Configuração da IDE de deploy automatizado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Segurança </t>
   </si>
   <si>
@@ -196,9 +191,6 @@
     <t>JPA</t>
   </si>
   <si>
-    <t>Java Spring / SpringBoot</t>
-  </si>
-  <si>
     <t>React, HTML, CSS, JS</t>
   </si>
   <si>
@@ -208,9 +200,6 @@
     <t>Notebooks, Desktops, Azure</t>
   </si>
   <si>
-    <t>Notebooks e dispositivos móveis, Windows, Linux, Firefox, Google Chrome, Microsoft Edge</t>
-  </si>
-  <si>
     <t>Metodologia SCRUM</t>
   </si>
   <si>
@@ -223,117 +212,9 @@
     <t>MySQL e PowerPoint</t>
   </si>
   <si>
-    <t>Visual Studio Code e IntelliJ</t>
-  </si>
-  <si>
     <t>GitHub (Definido pela faculdade)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">TesteCase + Ferramenta Jmeter </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">IIS Tomcat </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SSO Com Google </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Azure DevOps </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Se houver </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">SDK para IoT </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TXT com informações de erros </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(REVER)</t>
-    </r>
-  </si>
-  <si>
     <t>MySQL</t>
   </si>
   <si>
@@ -346,18 +227,12 @@
     <t>Adicionar diversas funcionalidades ao site e fazer a integração com diferentes aplicações: Redes sociais e Sistemas de pagamento.</t>
   </si>
   <si>
-    <t>Conexão com o dispositivo de Hardware.</t>
-  </si>
-  <si>
     <t>Mostrar mensagens de erros ou exceções.</t>
   </si>
   <si>
     <t>Classes de integração do Front End com a camada de acessos a dados e implementação de regras de negócios.</t>
   </si>
   <si>
-    <t>Encontrar e investigar bugs mais rapidamente, melhorar a qualidade do software e reduzir o tempo que leva para validar e lançar novas atualizações.</t>
-  </si>
-  <si>
     <t>Linguagens intuitivas e flexiveis.</t>
   </si>
   <si>
@@ -407,6 +282,39 @@
   </si>
   <si>
     <t>Documentação do projeto contendo todo escopo, estrutura e andamento do mesmo.</t>
+  </si>
+  <si>
+    <t>Criptografia de senhas e documentos pessoais</t>
+  </si>
+  <si>
+    <t>Tratamento de exceções, (try catch)</t>
+  </si>
+  <si>
+    <t>Não usaremos.</t>
+  </si>
+  <si>
+    <t>Backend / SpringBoot</t>
+  </si>
+  <si>
+    <t>não usaremos.</t>
+  </si>
+  <si>
+    <t>Azure DevOps</t>
+  </si>
+  <si>
+    <t>Configuração da IDE de deploy automatizado / GITHUB</t>
+  </si>
+  <si>
+    <t>IIS</t>
+  </si>
+  <si>
+    <t>Notebooks e dispositivos móveis, Windows, Linux, Firefox, Google Chrome, Microsoft Edge, Opera</t>
+  </si>
+  <si>
+    <t>Visual Studio Code, IntelliJ e Azure Data Studio</t>
+  </si>
+  <si>
+    <t>TesteCase + Ferramenta Jmeter</t>
   </si>
 </sst>
 </file>
@@ -608,44 +516,44 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,15 +837,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036DB22A-6FFA-4CD0-A3AA-AF0DD32AFF0D}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="56" style="1"/>
   </cols>
   <sheetData>
@@ -946,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" thickBot="1">
+    <row r="2" spans="1:5" ht="16.5" thickBot="1">
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:5">
@@ -965,353 +873,349 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>73</v>
+      <c r="D4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5">
+      <c r="A6" s="19"/>
+      <c r="B6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5">
+      <c r="A7" s="19"/>
+      <c r="B7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="31.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="31.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.25" customHeight="1">
+      <c r="A8" s="19"/>
+      <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5">
+      <c r="A10" s="19"/>
+      <c r="B10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="E10" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="19"/>
+      <c r="B11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31.5">
+      <c r="A12" s="19"/>
+      <c r="B12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="19"/>
+      <c r="B13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="46.8">
-      <c r="A9" s="8"/>
-      <c r="B9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="31.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="46.8">
-      <c r="A11" s="8"/>
-      <c r="B11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="31.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" ht="31.2">
-      <c r="A15" s="8" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" ht="31.5">
+      <c r="A15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5">
+      <c r="A16" s="19"/>
+      <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="31.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="31.5">
+      <c r="A17" s="19"/>
+      <c r="B17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="31.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="16" t="s">
+      <c r="C17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="D17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="31.5">
+      <c r="A18" s="19"/>
+      <c r="B18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="D18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="31.5">
+      <c r="A19" s="19"/>
+      <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="31.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>88</v>
+      <c r="D19" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="1:5" ht="46.8">
-      <c r="A21" s="8" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="47.25">
+      <c r="A21" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="47.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="C22" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="31.5">
+      <c r="A23" s="19"/>
+      <c r="B23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="19"/>
+      <c r="B24" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="46.8">
-      <c r="A22" s="8"/>
-      <c r="B22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="E24" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="31.5">
+      <c r="A25" s="19"/>
+      <c r="B25" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="31.5">
+      <c r="A26" s="19"/>
+      <c r="B26" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="31.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="8"/>
-      <c r="B24" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="31.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="31.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="13" t="s">
+      <c r="E26" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="32.25" thickBot="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="C27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="31.8" thickBot="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>94</v>
+      <c r="E27" s="18" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:5">

</xml_diff>

<commit_message>
Alterações no desenho de arquitetura
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de arquitetura.xlsx
+++ b/Documentação/Planilha de arquitetura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41CBBE3F-8E1F-45BE-A5D2-3953200CD16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F8F5A-A608-4322-A922-A22469A6E465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guia de Engenharia v4" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
   <si>
     <t>O que é crítico na sua aplicação? O que gera alto impacto?</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>Backend / SpringBoot</t>
-  </si>
-  <si>
-    <t>não usaremos.</t>
   </si>
   <si>
     <t>Azure DevOps</t>
@@ -837,15 +834,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036DB22A-6FFA-4CD0-A3AA-AF0DD32AFF0D}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
     <col min="4" max="16384" width="56" style="1"/>
   </cols>
   <sheetData>
@@ -854,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1">
+    <row r="2" spans="1:5" ht="16.2" thickBot="1">
       <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:5">
@@ -904,7 +901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.5">
+    <row r="6" spans="1:5" ht="31.2">
       <c r="A6" s="19"/>
       <c r="B6" s="11" t="s">
         <v>10</v>
@@ -919,7 +916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5">
+    <row r="7" spans="1:5" ht="31.2">
       <c r="A7" s="19"/>
       <c r="B7" s="11" t="s">
         <v>12</v>
@@ -947,7 +944,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="47.25">
+    <row r="9" spans="1:5" ht="46.8">
       <c r="A9" s="19"/>
       <c r="B9" s="11" t="s">
         <v>16</v>
@@ -962,7 +959,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="31.5">
+    <row r="10" spans="1:5" ht="31.2">
       <c r="A10" s="19"/>
       <c r="B10" s="11" t="s">
         <v>17</v>
@@ -987,19 +984,19 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="31.5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="31.2">
       <c r="A12" s="19"/>
       <c r="B12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>68</v>
@@ -1027,7 +1024,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" ht="31.5">
+    <row r="15" spans="1:5" ht="31.2">
       <c r="A15" s="19" t="s">
         <v>24</v>
       </c>
@@ -1044,7 +1041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.5">
+    <row r="16" spans="1:5" ht="31.2">
       <c r="A16" s="19"/>
       <c r="B16" s="11" t="s">
         <v>27</v>
@@ -1059,7 +1056,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="31.5">
+    <row r="17" spans="1:5" ht="31.2">
       <c r="A17" s="19"/>
       <c r="B17" s="14" t="s">
         <v>29</v>
@@ -1068,13 +1065,13 @@
         <v>30</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="31.5">
+    <row r="18" spans="1:5" ht="31.2">
       <c r="A18" s="19"/>
       <c r="B18" s="14" t="s">
         <v>31</v>
@@ -1089,7 +1086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="31.5">
+    <row r="19" spans="1:5" ht="31.2">
       <c r="A19" s="19"/>
       <c r="B19" s="14" t="s">
         <v>33</v>
@@ -1098,7 +1095,7 @@
         <v>34</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>75</v>
@@ -1111,7 +1108,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" ht="47.25">
+    <row r="21" spans="1:5" ht="46.8">
       <c r="A21" s="19" t="s">
         <v>35</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="47.25">
+    <row r="22" spans="1:5" ht="46.8">
       <c r="A22" s="19"/>
       <c r="B22" s="14" t="s">
         <v>38</v>
@@ -1143,7 +1140,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="31.5">
+    <row r="23" spans="1:5" ht="31.2">
       <c r="A23" s="19"/>
       <c r="B23" s="14" t="s">
         <v>40</v>
@@ -1173,7 +1170,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="31.5">
+    <row r="25" spans="1:5" ht="31.2">
       <c r="A25" s="19"/>
       <c r="B25" s="14" t="s">
         <v>44</v>
@@ -1182,13 +1179,13 @@
         <v>45</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="31.5">
+    <row r="26" spans="1:5" ht="31.2">
       <c r="A26" s="19"/>
       <c r="B26" s="11" t="s">
         <v>46</v>
@@ -1203,7 +1200,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="32.25" thickBot="1">
+    <row r="27" spans="1:5" ht="31.8" thickBot="1">
       <c r="A27" s="20"/>
       <c r="B27" s="17" t="s">
         <v>48</v>
@@ -1212,7 +1209,7 @@
         <v>49</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Planilha de arquitetura atualizada
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de arquitetura.xlsx
+++ b/Documentação/Planilha de arquitetura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facul\PROJETO PI DREAM HOUSE\Documentação do projeto\Documentos\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F8F5A-A608-4322-A922-A22469A6E465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B15665-AFB8-4B53-B5EE-9BA97D6A90C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guia de Engenharia v4" sheetId="3" r:id="rId1"/>
@@ -209,9 +209,6 @@
     <t>Planner</t>
   </si>
   <si>
-    <t>MySQL e PowerPoint</t>
-  </si>
-  <si>
     <t>GitHub (Definido pela faculdade)</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>Garantir mais segurança na autenticação do usuário.</t>
   </si>
   <si>
-    <t>Wi-fi, 3G, 4G, 5G</t>
-  </si>
-  <si>
     <t>Conexão de WI-FI e redes de dados</t>
   </si>
   <si>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>TesteCase + Ferramenta Jmeter</t>
+  </si>
+  <si>
+    <t>Conexão com a internet</t>
+  </si>
+  <si>
+    <t>Workbench e PowerPoint</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036DB22A-6FFA-4CD0-A3AA-AF0DD32AFF0D}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.6"/>
@@ -880,13 +880,13 @@
         <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="46.8">
       <c r="A5" s="19"/>
       <c r="B5" s="11" t="s">
         <v>8</v>
@@ -898,7 +898,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.2">
@@ -910,10 +910,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="31.2">
@@ -928,7 +928,7 @@
         <v>51</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1">
@@ -941,7 +941,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="46.8">
@@ -950,13 +950,13 @@
         <v>16</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.2">
@@ -971,7 +971,7 @@
         <v>52</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -984,7 +984,7 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31.2">
@@ -993,13 +993,13 @@
         <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1011,10 +1011,10 @@
         <v>23</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1035,10 +1035,10 @@
         <v>26</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.2">
@@ -1053,7 +1053,7 @@
         <v>53</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31.2">
@@ -1065,10 +1065,10 @@
         <v>30</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="31.2">
@@ -1083,7 +1083,7 @@
         <v>54</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="31.2">
@@ -1095,10 +1095,10 @@
         <v>34</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1122,7 +1122,7 @@
         <v>55</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="46.8">
@@ -1137,7 +1137,7 @@
         <v>56</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.2">
@@ -1152,7 +1152,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1164,10 +1164,10 @@
         <v>43</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="31.2">
@@ -1179,10 +1179,10 @@
         <v>45</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.2">
@@ -1194,10 +1194,10 @@
         <v>47</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="31.8" thickBot="1">
@@ -1209,10 +1209,10 @@
         <v>49</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5">

</xml_diff>